<commit_message>
feat: listo para revision
</commit_message>
<xml_diff>
--- a/assets/ExcelAppDesign.xlsx
+++ b/assets/ExcelAppDesign.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/x399499/Documents/Fictizia/MagicsImprover/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5C9ADB-CBA8-734C-81C1-41FBC0C12F62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4452DDFF-9623-A34F-884F-D1CEFD673CB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{76C21FD5-664E-6348-8CE9-C70BCFDCBF62}"/>
   </bookViews>
@@ -310,8 +310,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="533400" y="1219200"/>
-          <a:ext cx="4102100" cy="5207000"/>
+          <a:off x="533400" y="1354667"/>
+          <a:ext cx="4123267" cy="5207000"/>
         </a:xfrm>
         <a:prstGeom prst="round2DiagRect">
           <a:avLst/>
@@ -357,16 +357,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>541867</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>118534</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -381,8 +381,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20015200" y="1816100"/>
-          <a:ext cx="5359400" cy="4876800"/>
+          <a:off x="51985334" y="1460500"/>
+          <a:ext cx="5384800" cy="4876800"/>
         </a:xfrm>
         <a:prstGeom prst="snip2DiagRect">
           <a:avLst/>
@@ -893,74 +893,6 @@
             <a:rPr lang="es-ES_tradnl" sz="1100"/>
             <a:t>LOGO		HOME			WORLD</a:t>
           </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>795867</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>186267</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>169334</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Rectángulo 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D21F291F-122D-1E47-A330-02EB157C72B2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11582400" y="355600"/>
-          <a:ext cx="6028267" cy="423334"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1100"/>
-            <a:t>CARD</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1100" baseline="0"/>
-            <a:t> SEARCHER				FILTERS</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3606,7 +3538,1562 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>389467</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>16934</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>67732</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="CuadroTexto 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F84846B-5E87-4C4B-BB5A-97CDDCEAFB21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20303067" y="152400"/>
+          <a:ext cx="5435600" cy="21386799"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "object": "card",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "id": "59d1f05b-f165-47c7-8a78-3b60ee3298ca",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "oracle_id": "f4aa8391-34d5-4ad2-a981-9aa08f8229db",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "multiverse_ids": [</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                8437</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            ],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "mtgo_id": 12459,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "mtgo_foil_id": 12460,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "tcgplayer_id": 6772,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "cardmarket_id": 10209,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "name": "Absolute Law",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "lang": "en",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "released_at": "1998-10-12",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "uri": "https://api.scryfall.com/cards/59d1f05b-f165-47c7-8a78-3b60ee3298ca",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "scryfall_uri": "https://scryfall.com/card/usg/2/absolute-law?utm_source=api",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "layout": "normal",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "highres_image": true,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "image_uris": {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "small": "https://c1.scryfall.com/file/scryfall-cards/small/front/5/9/59d1f05b-f165-47c7-8a78-3b60ee3298ca.jpg?1562913728",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "normal": "https://c1.scryfall.com/file/scryfall-cards/normal/front/5/9/59d1f05b-f165-47c7-8a78-3b60ee3298ca.jpg?1562913728",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "large": "https://c1.scryfall.com/file/scryfall-cards/large/front/5/9/59d1f05b-f165-47c7-8a78-3b60ee3298ca.jpg?1562913728",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "png": "https://c1.scryfall.com/file/scryfall-cards/png/front/5/9/59d1f05b-f165-47c7-8a78-3b60ee3298ca.png?1562913728",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "art_crop": "https://c1.scryfall.com/file/scryfall-cards/art_crop/front/5/9/59d1f05b-f165-47c7-8a78-3b60ee3298ca.jpg?1562913728",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "border_crop": "https://c1.scryfall.com/file/scryfall-cards/border_crop/front/5/9/59d1f05b-f165-47c7-8a78-3b60ee3298ca.jpg?1562913728"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            },</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "mana_cost": "{1}{W}",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "cmc": 2.0,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "type_line": "Enchantment",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "oracle_text": "All creatures have protection from red.",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "colors": [</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "W"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            ],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "color_identity": [</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "W"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            ],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "keywords": [],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "legalities": {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "standard": "not_legal",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "future": "not_legal",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "historic": "not_legal",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "pioneer": "not_legal",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "modern": "not_legal",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "legacy": "legal",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "pauper": "not_legal",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "vintage": "legal",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "penny": "not_legal",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "commander": "legal",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "brawl": "not_legal",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "duel": "legal",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "oldschool": "not_legal"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            },</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "games": [</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "paper",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "mtgo"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            ],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "reserved": false,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "foil": false,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "nonfoil": true,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "oversized": false,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "promo": false,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "reprint": false,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "variation": false,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "set": "usg",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "set_name": "Urza's Saga",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "set_type": "expansion",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "set_uri": "https://api.scryfall.com/sets/c330df40-51db-4caf-bde6-48df6c181001",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "set_search_uri": "https://api.scryfall.com/cards/search?order=set&amp;q=e%3Ausg&amp;unique=prints",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "scryfall_set_uri": "https://scryfall.com/sets/usg?utm_source=api",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "rulings_uri": "https://api.scryfall.com/cards/59d1f05b-f165-47c7-8a78-3b60ee3298ca/rulings",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "prints_search_uri": "https://api.scryfall.com/cards/search?order=released&amp;q=oracleid%3Af4aa8391-34d5-4ad2-a981-9aa08f8229db&amp;unique=prints",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "collector_number": "2",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "digital": false,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "rarity": "uncommon",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "flavor_text": "The strength of law is unwavering. It is an iron bar in a world of water.",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "card_back_id": "0aeebaf5-8c7d-4636-9e82-8c27447861f7",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "artist": "Mark Zug",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "artist_ids": [</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "48e2b98c-5467-4671-bd42-4c3746115117"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            ],</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "illustration_id": "951f849e-b0ba-4cda-9fdc-d6cbca84f840",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "border_color": "black",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "frame": "1997",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "full_art": false,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "textless": false,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "booster": true,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "story_spotlight": false,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "edhrec_rank": 13072,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "prices": {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "usd": "0.41",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "usd_foil": null,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "eur": "0.34",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "eur_foil": null,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "tix": "0.10"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            },</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "related_uris": {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "gatherer": "https://gatherer.wizards.com/Pages/Card/Details.aspx?multiverseid=8437",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "tcgplayer_decks": "https://decks.tcgplayer.com/magic/deck/search?contains=Absolute+Law&amp;page=1&amp;utm_campaign=affiliate&amp;utm_medium=api&amp;utm_source=scryfall",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "edhrec": "https://edhrec.com/route/?cc=Absolute+Law",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "mtgtop8": "https://mtgtop8.com/search?MD_check=1&amp;SB_check=1&amp;cards=Absolute+Law"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            },</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            "purchase_uris": {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "tcgplayer": "https://shop.tcgplayer.com/product/productsearch?id=6772&amp;utm_campaign=affiliate&amp;utm_medium=api&amp;utm_source=scryfall",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "cardmarket": "https://www.cardmarket.com/en/Magic/Products/Singles/Urzas-Saga/Absolute-Law?referrer=scryfall&amp;utm_campaign=card_prices&amp;utm_medium=text&amp;utm_source=scryfall",</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                "cardhoarder": "https://www.cardhoarder.com/cards/12459?affiliate_id=scryfall&amp;ref=card-profile&amp;utm_campaign=affiliate&amp;utm_medium=card&amp;utm_source=scryfall"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        },</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES_tradnl" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3908,8 +5395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84232087-9323-C14B-8CA2-5F51AE3E4659}">
   <dimension ref="J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="75" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" workbookViewId="0">
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>